<commit_message>
feat(ViewUser) : page cree
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B55C284-7AE8-4C7A-BA43-D53BC4E36110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C9C65C-BC42-45C9-A4F9-290E26AB9690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Commencer le frontend</t>
+  </si>
+  <si>
+    <t>Impossible de charger le frontend, doit faire les branches, le docker</t>
+  </si>
+  <si>
+    <t>Commencer la page UserView</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1076,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1088,7 +1094,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,7 +2007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2060,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 30 minutes</v>
+        <v>0 jours 3 heurs 20 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2069,15 +2075,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2238,15 +2244,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
+        <v>15</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45756</v>
+      </c>
+      <c r="C12" s="47">
+        <v>1</v>
+      </c>
       <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2259,15 +2273,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45756</v>
+      </c>
       <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="52">
+        <v>50</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -8643,7 +8665,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8651,7 +8673,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>2.0833333333333332E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8747,7 +8769,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
@@ -8759,7 +8781,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8768,7 +8790,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>6.2499999999999993E-2</v>
+        <v>0.13888888888888887</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8791,6 +8813,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9013,17 +9046,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9033,6 +9055,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9049,15 +9082,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(LivreCard) : Css de la page d'acceuil
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3EC666-AFFB-4F95-BA5A-0B005D606A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE06FBC5-94FE-4359-A795-33D486083A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>Fait les images, et la page userView</t>
+  </si>
+  <si>
+    <t>Mit les images</t>
+  </si>
+  <si>
+    <t>Fait le Css de la page d'acceuil</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1088,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.375E-2</c:v>
+                  <c:v>0.21875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2013,7 +2019,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="1" sqref="A15:F16 F24"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2066,7 +2072,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 4 heurs 15 minutes</v>
+        <v>0 jours 7 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2081,15 +2087,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>195</v>
+        <v>255</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>255</v>
+        <v>435</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2396,30 +2402,48 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45777</v>
+      </c>
       <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="D18" s="48">
+        <v>20</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45777</v>
+      </c>
+      <c r="C19" s="51">
+        <v>2</v>
+      </c>
+      <c r="D19" s="52">
+        <v>40</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
@@ -8683,11 +8707,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8695,7 +8719,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>9.375E-2</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8812,7 +8836,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.17708333333333331</v>
+        <v>0.30208333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8835,6 +8859,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9057,17 +9092,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9077,6 +9101,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9093,15 +9128,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore (Journal) : Fait le journal
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE06FBC5-94FE-4359-A795-33D486083A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF387D0-C76C-4419-8098-E9778851E468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Fait le Css de la page d'acceuil</t>
+  </si>
+  <si>
+    <t>Continuer le Css du site</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1091,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21875</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2019,7 +2022,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2075,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 15 minutes</v>
+        <v>0 jours 9 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2087,15 +2090,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>435</v>
+        <v>570</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2462,15 +2465,25 @@
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45783</v>
+      </c>
+      <c r="C21" s="51">
+        <v>2</v>
+      </c>
+      <c r="D21" s="52">
+        <v>15</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2506,7 +2519,9 @@
       <c r="C24" s="47"/>
       <c r="D24" s="48"/>
       <c r="E24" s="49"/>
-      <c r="F24" s="36"/>
+      <c r="F24" s="36">
+        <v>135</v>
+      </c>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -8707,11 +8722,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8719,7 +8734,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.21875</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8836,7 +8851,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.30208333333333337</v>
+        <v>0.39583333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8859,17 +8874,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9092,6 +9096,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9101,17 +9116,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9128,4 +9132,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UX (Css) : Css uniformise
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF387D0-C76C-4419-8098-E9778851E468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E68571-1830-4763-806C-A186ECCEA806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="10050" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Continuer le Css du site</t>
+  </si>
+  <si>
+    <t>regler les problemes d'affichage</t>
+  </si>
+  <si>
+    <t>Refait certains vue et presque fini le frontend</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1097,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3125</c:v>
+                  <c:v>0.4375</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2021,8 +2027,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2075,7 +2081,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 30 minutes</v>
+        <v>0 jours 12 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2090,7 +2096,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2098,7 +2104,7 @@
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>570</v>
+        <v>750</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2499,28 +2505,42 @@
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="str">
+      <c r="A23" s="16">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="50">
+        <v>45784</v>
+      </c>
+      <c r="C23" s="51">
+        <v>2</v>
+      </c>
       <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="36"/>
+      <c r="E23" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="46">
+        <v>45784</v>
+      </c>
+      <c r="C24" s="47">
+        <v>1</v>
+      </c>
       <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="36">
-        <v>135</v>
+      <c r="E24" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>41</v>
       </c>
       <c r="G24" s="55"/>
     </row>
@@ -8722,7 +8742,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>420</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8734,7 +8754,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.3125</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8851,7 +8871,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.39583333333333337</v>
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8874,6 +8894,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9096,17 +9127,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9116,6 +9136,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9132,15 +9163,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UX(Style générale) : organiser le main.css et rajouter les style scoped
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A8924F-9B4F-4E74-A670-80A985715C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AFACB-88CE-4936-8AD6-3EE2110E2E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="11415" yWindow="1005" windowWidth="23400" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Page de modifications en cours</t>
+  </si>
+  <si>
+    <t>Page de modifications fini</t>
+  </si>
+  <si>
+    <t>Finitions de Css, mettre ce qu'il faut en scoped</t>
+  </si>
+  <si>
+    <t>Reçu des notes</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1109,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59375</c:v>
+                  <c:v>0.73611111111111116</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1109,7 +1118,7 @@
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3888888888888888E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2030,8 +2039,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2093,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 16 heurs 15 minutes</v>
+        <v>0 jours 20 heurs 0 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2099,15 +2108,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>660</v>
+        <v>840</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>975</v>
+        <v>1200</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2582,39 +2591,67 @@
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="str">
+      <c r="A27" s="16">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B27" s="50">
+        <v>45797</v>
+      </c>
       <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="52">
+        <v>20</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>45</v>
+      </c>
       <c r="G27" s="56"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45797</v>
+      </c>
+      <c r="C28" s="47">
+        <v>2</v>
+      </c>
+      <c r="D28" s="48">
+        <v>10</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="str">
+      <c r="A29" s="16">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B29" s="50">
+        <v>45797</v>
+      </c>
+      <c r="C29" s="51">
+        <v>1</v>
+      </c>
+      <c r="D29" s="52">
+        <v>15</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>44</v>
+      </c>
       <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8755,11 +8792,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>600</v>
+        <v>780</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8767,7 +8804,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.59375</v>
+        <v>0.73611111111111116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8813,7 +8850,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8821,7 +8858,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>1.3888888888888888E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8884,7 +8921,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.67708333333333326</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore(Journal) : fait mon journal
</commit_message>
<xml_diff>
--- a/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
+++ b/Journaux/Journal-de-Travail_ThomasMoreira.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_WEB295\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8A751B-4D50-4BD8-ABEF-7C9988CD677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C79F6B5-87C5-4481-9DF8-548B7DE500AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="11415" yWindow="1005" windowWidth="23400" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>Commencer le rapport</t>
+  </si>
+  <si>
+    <t>Continuer le rapport</t>
+  </si>
+  <si>
+    <t>Présentation du projet au prof</t>
+  </si>
+  <si>
+    <t>Finit le rapport</t>
+  </si>
+  <si>
+    <t>Travailler sur d'autres projet</t>
   </si>
 </sst>
 </file>
@@ -1124,19 +1136,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9444444444444448E-2</c:v>
+                  <c:v>0.1736111111111111</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2048,8 +2060,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2102,7 +2114,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 23 heurs 0 minutes</v>
+        <v>1 jours 2 heurs 44 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2117,15 +2129,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>960</v>
+        <v>1140</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>420</v>
+        <v>465</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1380</v>
+        <v>1605</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2750,51 +2762,89 @@
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="str">
+      <c r="A35" s="16">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="36"/>
+        <v>22</v>
+      </c>
+      <c r="B35" s="50">
+        <v>45804</v>
+      </c>
+      <c r="C35" s="51">
+        <v>1</v>
+      </c>
+      <c r="D35" s="52">
+        <v>30</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="G35" s="56"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="str">
+      <c r="A36" s="8">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B36" s="46">
+        <v>45804</v>
+      </c>
       <c r="C36" s="47"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="35"/>
+      <c r="D36" s="48">
+        <v>15</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="G36" s="55"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="str">
+      <c r="A37" s="16">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="B37" s="50">
+        <v>45804</v>
+      </c>
+      <c r="C37" s="51">
+        <v>1</v>
+      </c>
+      <c r="D37" s="52">
+        <v>0</v>
+      </c>
+      <c r="E37" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="G37" s="56"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="str">
+      <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="B38" s="46">
+        <v>45804</v>
+      </c>
+      <c r="C38" s="47">
+        <v>1</v>
+      </c>
+      <c r="D38" s="48">
+        <v>0</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>52</v>
+      </c>
       <c r="G38" s="55"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -8863,11 +8913,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8875,7 +8925,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>6.9444444444444448E-2</v>
+        <v>0.1736111111111111</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8903,7 +8953,7 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C9" s="31" t="str">
         <f>'Journal de travail'!M13</f>
@@ -8911,7 +8961,7 @@
       </c>
       <c r="D9" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -8935,7 +8985,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
@@ -8947,7 +8997,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8956,7 +9006,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.95833333333333326</v>
+        <v>1.1145833333333333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8979,17 +9029,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9212,6 +9251,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9221,17 +9271,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9248,4 +9287,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>